<commit_message>
Update code -> New Instructions added to README. Set up of venv, Distribution
</commit_message>
<xml_diff>
--- a/DatabaseFolder/mastermodels_database.xlsx
+++ b/DatabaseFolder/mastermodels_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\MasterModelAutomation by Zovinec\AutomationApp\DatabaseFolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\AutomationApp\DatabaseFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7EE7A2-6547-4342-BABF-D520865EBA90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74D266E-95C3-4A9A-8A1F-EC880E35DA77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{1BE75684-FFFF-4349-8575-C46FEBD2E57E}"/>
+    <workbookView xWindow="26805" yWindow="2745" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{1BE75684-FFFF-4349-8575-C46FEBD2E57E}"/>
   </bookViews>
   <sheets>
     <sheet name="CX" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="35">
   <si>
     <t>CAD mastermodel name</t>
   </si>
@@ -218,6 +218,21 @@
   </si>
   <si>
     <t>0651</t>
+  </si>
+  <si>
+    <t>endofsheet</t>
+  </si>
+  <si>
+    <t>SecondaryPP</t>
+  </si>
+  <si>
+    <t>cx_0250_emptyy.asm</t>
+  </si>
+  <si>
+    <t>cx_0250_gm1811.asm</t>
+  </si>
+  <si>
+    <t>END_OF_WORKSHEET</t>
   </si>
 </sst>
 </file>
@@ -682,10 +697,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B9A276-C1BD-4799-B4E6-E23DC5267C1F}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" style="3" customWidth="1"/>
+    <col min="2" max="7" width="20.7109375" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="20.7109375" style="4" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E09D66-4249-4D9E-83BC-2B3AF14AAB1A}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +826,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
@@ -794,124 +903,10 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E09D66-4249-4D9E-83BC-2B3AF14AAB1A}">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.28515625" style="3" customWidth="1"/>
-    <col min="2" max="6" width="20.7109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="20.7109375" style="4" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -923,7 +918,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,7 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3017E54F-5BBF-4D12-80F3-FA52B25B0DF9}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>